<commit_message>
Added piezo transducer.  Working on footprints
</commit_message>
<xml_diff>
--- a/hardware/beer-gauge-bom.xlsx
+++ b/hardware/beer-gauge-bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="139">
   <si>
     <t>Ref</t>
   </si>
@@ -325,9 +325,6 @@
     <t>Y2</t>
   </si>
   <si>
-    <t>32.768kHz</t>
-  </si>
-  <si>
     <t>CAP ALUM 220UF 20% 10V SMD</t>
   </si>
   <si>
@@ -414,6 +411,30 @@
   </si>
   <si>
     <t>Crystals:Crystal_SMD_2520_4Pads</t>
+  </si>
+  <si>
+    <t>32.768kHz ±20ppm Crystal 12.5pF</t>
+  </si>
+  <si>
+    <t>535-9542-1-ND</t>
+  </si>
+  <si>
+    <t>footprint:ABS07</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>BUZZER PIEZO 12.5V 9MM SMD</t>
+  </si>
+  <si>
+    <t>490-9647-1-ND</t>
+  </si>
+  <si>
+    <t>R1,R4</t>
+  </si>
+  <si>
+    <t>1k</t>
   </si>
 </sst>
 </file>
@@ -770,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -816,27 +837,27 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>104</v>
-      </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="29">
       <c r="B4" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -848,27 +869,27 @@
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
         <v>110</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>111</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:8">
@@ -876,19 +897,19 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>114</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -896,19 +917,19 @@
         <v>98</v>
       </c>
       <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
         <v>118</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>119</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="2:8">
@@ -950,22 +971,22 @@
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>122</v>
-      </c>
       <c r="F14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -973,153 +994,194 @@
         <v>97</v>
       </c>
       <c r="C15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
         <v>123</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>124</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="2:8">
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>138</v>
+      </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>126</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>127</v>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>105</v>
-      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>6</v>
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>131</v>
+        <v>106</v>
+      </c>
+      <c r="H24" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" t="s">
         <v>101</v>
       </c>
-      <c r="C25" t="s">
-        <v>102</v>
+      <c r="C28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on capacitive touch pad.  Added footprint for piezo
</commit_message>
<xml_diff>
--- a/hardware/beer-gauge-bom.xlsx
+++ b/hardware/beer-gauge-bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="147">
   <si>
     <t>Ref</t>
   </si>
@@ -434,7 +434,31 @@
     <t>R1,R4</t>
   </si>
   <si>
-    <t>1k</t>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>HOLDER COIN CELL 12MM SMD</t>
+  </si>
+  <si>
+    <t>BK-885-CT-ND</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>568-6524-1-ND</t>
+  </si>
+  <si>
+    <t>DIODE ARRAY SCHOTTKY 40V 3HUSON</t>
+  </si>
+  <si>
+    <t>footprint:PKMCS</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-1.00KHRCT-ND</t>
   </si>
 </sst>
 </file>
@@ -791,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H28"/>
+  <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -834,353 +858,412 @@
     </row>
     <row r="3" spans="2:8">
       <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>102</v>
+        <v>138</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="29">
-      <c r="B4" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>108</v>
-      </c>
+      <c r="E3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="29">
+      <c r="B6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="D13" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>119</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17">
         <v>2</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G17" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" t="s">
         <v>134</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
         <v>136</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>125</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>126</v>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>104</v>
-      </c>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="2:8">
       <c r="B23" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
-        <v>106</v>
-      </c>
-      <c r="H24" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>107</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>6</v>
+        <v>82</v>
+      </c>
+      <c r="D27" t="s">
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>130</v>
+        <v>106</v>
+      </c>
+      <c r="H27" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" t="s">
         <v>101</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>131</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
         <v>132</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added footprint for coin cell battery holder and RJ10 jack
</commit_message>
<xml_diff>
--- a/hardware/beer-gauge-bom.xlsx
+++ b/hardware/beer-gauge-bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="149">
   <si>
     <t>Ref</t>
   </si>
@@ -459,6 +459,12 @@
   </si>
   <si>
     <t>311-1.00KHRCT-ND</t>
+  </si>
+  <si>
+    <t>footprint:BK-885</t>
+  </si>
+  <si>
+    <t>footprint:0855135016</t>
   </si>
 </sst>
 </file>
@@ -818,7 +824,7 @@
   <dimension ref="B2:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -872,7 +878,9 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8">
@@ -1016,6 +1024,9 @@
       </c>
       <c r="F14">
         <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="2:8">

</xml_diff>

<commit_message>
Working on footprints.  Exported netlist into layout.
</commit_message>
<xml_diff>
--- a/hardware/beer-gauge-bom.xlsx
+++ b/hardware/beer-gauge-bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="153">
   <si>
     <t>Ref</t>
   </si>
@@ -301,12 +301,6 @@
     <t>P5</t>
   </si>
   <si>
-    <t>USB - mini B USB 2.0 OTG</t>
-  </si>
-  <si>
-    <t>WM17116CT-ND</t>
-  </si>
-  <si>
     <t>https://www.pjrc.com/store/ic_mkl02.html</t>
   </si>
   <si>
@@ -465,6 +459,24 @@
   </si>
   <si>
     <t>footprint:0855135016</t>
+  </si>
+  <si>
+    <t>USB - micro B USB 2.0 Receptacle</t>
+  </si>
+  <si>
+    <t>609-4613-1-ND</t>
+  </si>
+  <si>
+    <t>footprint:10118192</t>
+  </si>
+  <si>
+    <t>footprint:SOT1061</t>
+  </si>
+  <si>
+    <t>CONN FPC BOTTOM 20POS 1.00MM R/A</t>
+  </si>
+  <si>
+    <t>WM7946CT-ND</t>
   </si>
 </sst>
 </file>
@@ -821,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H31"/>
+  <dimension ref="B2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -864,22 +876,22 @@
     </row>
     <row r="3" spans="2:8">
       <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -897,27 +909,27 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="29">
       <c r="B6" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -929,27 +941,27 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7">
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -957,179 +969,182 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>112</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" t="s">
         <v>141</v>
       </c>
-      <c r="C10" t="s">
-        <v>143</v>
-      </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
+      <c r="G10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>119</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" t="s">
         <v>90</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
         <v>92</v>
       </c>
-      <c r="F14">
+      <c r="F16">
         <v>4</v>
       </c>
-      <c r="G14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8">
-      <c r="B15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="D16" s="2"/>
+      <c r="G16" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>123</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18" t="s">
-        <v>119</v>
-      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" t="s">
-        <v>55</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="2:8">
-      <c r="D20" s="2"/>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" t="s">
-        <v>134</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -1137,145 +1152,168 @@
     </row>
     <row r="23" spans="2:8">
       <c r="B23" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>126</v>
-      </c>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" t="s">
-        <v>81</v>
+        <v>88</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>106</v>
-      </c>
-      <c r="H27" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>104</v>
+      </c>
+      <c r="H29" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="2:8">
       <c r="B30" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
         <v>128</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" t="s">
         <v>129</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="31" spans="2:8">
-      <c r="B31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
         <v>131</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished footprints.  Switched to a tantalum cap for the LCD.  Changed piezo resistor value to 470 to reduce part count.
</commit_message>
<xml_diff>
--- a/hardware/beer-gauge-bom.xlsx
+++ b/hardware/beer-gauge-bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="154">
   <si>
     <t>Ref</t>
   </si>
@@ -319,12 +319,6 @@
     <t>Y2</t>
   </si>
   <si>
-    <t>CAP ALUM 220UF 20% 10V SMD</t>
-  </si>
-  <si>
-    <t>P15084CT-ND</t>
-  </si>
-  <si>
     <t>Housings_SSOP:TSSOP-28_4.4x9.7mm_Pitch0.65mm</t>
   </si>
   <si>
@@ -395,9 +389,6 @@
     <t>Buttons_Switches_SMD:SW_SPST_KMR2</t>
   </si>
   <si>
-    <t>Capacitors_SMD:c_elec_6.3x5.8</t>
-  </si>
-  <si>
     <t>16MHz ±15ppm Crystal 8pF</t>
   </si>
   <si>
@@ -425,9 +416,6 @@
     <t>490-9647-1-ND</t>
   </si>
   <si>
-    <t>R1,R4</t>
-  </si>
-  <si>
     <t>BT1</t>
   </si>
   <si>
@@ -449,12 +437,6 @@
     <t>footprint:PKMCS</t>
   </si>
   <si>
-    <t>RES SMD 1K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>311-1.00KHRCT-ND</t>
-  </si>
-  <si>
     <t>footprint:BK-885</t>
   </si>
   <si>
@@ -477,6 +459,27 @@
   </si>
   <si>
     <t>WM7946CT-ND</t>
+  </si>
+  <si>
+    <t>CABLE FFC 1MM TYPE 2 20P100MM</t>
+  </si>
+  <si>
+    <t>732-5134-ND</t>
+  </si>
+  <si>
+    <t>R1,R4,R5</t>
+  </si>
+  <si>
+    <t>CAP TANT 220UF 16V 10% 2917</t>
+  </si>
+  <si>
+    <t>399-10429-1-ND</t>
+  </si>
+  <si>
+    <t>Capacitors_Tantalum_SMD:TantalC_SizeD_EIA-7343_Reflow</t>
+  </si>
+  <si>
+    <t>footprint:0522712069</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -531,6 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -833,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H33"/>
+  <dimension ref="B2:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -876,22 +880,22 @@
     </row>
     <row r="3" spans="2:8">
       <c r="B3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -909,27 +913,27 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="29">
       <c r="B6" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -941,27 +945,27 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F7">
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -969,39 +973,39 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>110</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="2:8">
@@ -1012,16 +1016,19 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F12">
         <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="2:8">
@@ -1029,19 +1036,19 @@
         <v>96</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F14">
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -1061,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:8">
@@ -1069,19 +1076,19 @@
         <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -1089,22 +1096,22 @@
     </row>
     <row r="19" spans="2:8">
       <c r="B19" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="2:8">
@@ -1112,173 +1119,173 @@
         <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>143</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>117</v>
-      </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="D22" s="2"/>
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C23" t="s">
-        <v>133</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>134</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>142</v>
-      </c>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" t="s">
+      <c r="B24" t="s">
         <v>97</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" t="s">
-        <v>124</v>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>6</v>
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="H28" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>104</v>
-      </c>
-      <c r="H29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8">
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
-        <v>85</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
         <v>126</v>
@@ -1296,24 +1303,24 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
-      <c r="B33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" t="s">
-        <v>129</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" t="s">
-        <v>130</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33" t="s">
-        <v>131</v>
+    <row r="34" spans="2:7">
+      <c r="B34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>148</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added RTC battery to BOM.  Fixed BOM quantities
</commit_message>
<xml_diff>
--- a/hardware/beer-gauge-bom.xlsx
+++ b/hardware/beer-gauge-bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="156">
   <si>
     <t>Ref</t>
   </si>
@@ -480,6 +480,12 @@
   </si>
   <si>
     <t>footprint:0522712069</t>
+  </si>
+  <si>
+    <t>BATTERY LITHIUM 3V COIN 12.5MM</t>
+  </si>
+  <si>
+    <t>P033-ND</t>
   </si>
 </sst>
 </file>
@@ -837,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H34"/>
+  <dimension ref="B2:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1025,7 +1031,7 @@
         <v>146</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
         <v>153</v>
@@ -1108,7 +1114,7 @@
         <v>117</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19" t="s">
         <v>115</v>
@@ -1319,8 +1325,23 @@
       <c r="F34">
         <v>1</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="6" t="s">
         <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating schematic/BOM to use 2 channel ADC, added I2C switch
</commit_message>
<xml_diff>
--- a/hardware/beer-gauge-bom.xlsx
+++ b/hardware/beer-gauge-bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="166">
   <si>
     <t>Ref</t>
   </si>
@@ -283,209 +283,239 @@
     <t>IC REG LDO 3.3V 0.5A 6WSON</t>
   </si>
   <si>
-    <t>IC ADC 24BIT BRDG SENSOR 28TSSOP</t>
-  </si>
-  <si>
-    <t>296-18673-5-ND</t>
+    <t>CONN MOD JACK 4P4C VERT UNSHLD</t>
+  </si>
+  <si>
+    <t>WM3555CT-ND</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>https://www.pjrc.com/store/ic_mkl02.html</t>
+  </si>
+  <si>
+    <t>R2,R3</t>
+  </si>
+  <si>
+    <t>L1-L3</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Housings_DFN_QFN:DFN-6-1EP_3x3mm_Pitch0.95mm</t>
+  </si>
+  <si>
+    <t>Housings_DFN_QFN:QFN-16-1EP_3x3mm_Pitch0.5mm</t>
+  </si>
+  <si>
+    <t>Housings_QFP:LQFP-64_10x10mm_Pitch0.5mm</t>
+  </si>
+  <si>
+    <t>Capacitors_SMD:C_0603</t>
+  </si>
+  <si>
+    <t>2.2µF ±10% 10V X7R Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>311-1797-1-ND</t>
+  </si>
+  <si>
+    <t>0.10µF ±10% 25V X7R Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>LED RED CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>754-1123-1-ND</t>
+  </si>
+  <si>
+    <t>LEDs:LED_0603</t>
+  </si>
+  <si>
+    <t>C5,C7,C8,C15</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 600 OHM 0603 1LN</t>
+  </si>
+  <si>
+    <t>490-1014-1-ND</t>
+  </si>
+  <si>
+    <t>Resistors_SMD:R_0603</t>
+  </si>
+  <si>
+    <t>RES SMD 470 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-470HRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 33 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-33.0HRCT-ND</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 32V</t>
+  </si>
+  <si>
+    <t>CKN10284CT-ND</t>
+  </si>
+  <si>
+    <t>Buttons_Switches_SMD:SW_SPST_KMR2</t>
+  </si>
+  <si>
+    <t>16MHz ±15ppm Crystal 8pF</t>
+  </si>
+  <si>
+    <t>644-1049-1-ND</t>
+  </si>
+  <si>
+    <t>Crystals:Crystal_SMD_2520_4Pads</t>
+  </si>
+  <si>
+    <t>32.768kHz ±20ppm Crystal 12.5pF</t>
+  </si>
+  <si>
+    <t>535-9542-1-ND</t>
+  </si>
+  <si>
+    <t>footprint:ABS07</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>BUZZER PIEZO 12.5V 9MM SMD</t>
+  </si>
+  <si>
+    <t>490-9647-1-ND</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>HOLDER COIN CELL 12MM SMD</t>
+  </si>
+  <si>
+    <t>BK-885-CT-ND</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>568-6524-1-ND</t>
+  </si>
+  <si>
+    <t>DIODE ARRAY SCHOTTKY 40V 3HUSON</t>
+  </si>
+  <si>
+    <t>footprint:PKMCS</t>
+  </si>
+  <si>
+    <t>footprint:BK-885</t>
+  </si>
+  <si>
+    <t>footprint:0855135016</t>
+  </si>
+  <si>
+    <t>USB - micro B USB 2.0 Receptacle</t>
+  </si>
+  <si>
+    <t>609-4613-1-ND</t>
+  </si>
+  <si>
+    <t>footprint:10118192</t>
+  </si>
+  <si>
+    <t>footprint:SOT1061</t>
+  </si>
+  <si>
+    <t>CONN FPC BOTTOM 20POS 1.00MM R/A</t>
+  </si>
+  <si>
+    <t>WM7946CT-ND</t>
+  </si>
+  <si>
+    <t>CABLE FFC 1MM TYPE 2 20P100MM</t>
+  </si>
+  <si>
+    <t>732-5134-ND</t>
+  </si>
+  <si>
+    <t>R1,R4,R5</t>
+  </si>
+  <si>
+    <t>CAP TANT 220UF 16V 10% 2917</t>
+  </si>
+  <si>
+    <t>399-10429-1-ND</t>
+  </si>
+  <si>
+    <t>Capacitors_Tantalum_SMD:TantalC_SizeD_EIA-7343_Reflow</t>
+  </si>
+  <si>
+    <t>footprint:0522712069</t>
+  </si>
+  <si>
+    <t>BATTERY LITHIUM 3V COIN 12.5MM</t>
+  </si>
+  <si>
+    <t>P033-ND</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>IC MULT-FUNCTION GATE SC70-6</t>
+  </si>
+  <si>
+    <t>296-15577-1-ND</t>
+  </si>
+  <si>
+    <t>TO_SOT_Packages_SMD:SC-70-6</t>
+  </si>
+  <si>
+    <t>C2-C4,C6,
+C9-C14,C16,C17</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-4.70KHRCT-ND</t>
   </si>
   <si>
     <t>P1-P4</t>
   </si>
   <si>
-    <t>CONN MOD JACK 4P4C VERT UNSHLD</t>
-  </si>
-  <si>
-    <t>WM3555CT-ND</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>https://www.pjrc.com/store/ic_mkl02.html</t>
-  </si>
-  <si>
-    <t>R2,R3</t>
-  </si>
-  <si>
-    <t>L1-L3</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>Y2</t>
-  </si>
-  <si>
-    <t>Housings_SSOP:TSSOP-28_4.4x9.7mm_Pitch0.65mm</t>
-  </si>
-  <si>
-    <t>Housings_DFN_QFN:DFN-6-1EP_3x3mm_Pitch0.95mm</t>
-  </si>
-  <si>
-    <t>Housings_DFN_QFN:QFN-16-1EP_3x3mm_Pitch0.5mm</t>
-  </si>
-  <si>
-    <t>Housings_QFP:LQFP-64_10x10mm_Pitch0.5mm</t>
-  </si>
-  <si>
-    <t>Capacitors_SMD:C_0603</t>
-  </si>
-  <si>
-    <t>2.2µF ±10% 10V X7R Ceramic Capacitor</t>
-  </si>
-  <si>
-    <t>311-1797-1-ND</t>
-  </si>
-  <si>
-    <t>0.10µF ±10% 25V X7R Ceramic Capacitor</t>
-  </si>
-  <si>
-    <t>LED RED CLEAR 0603 SMD</t>
-  </si>
-  <si>
-    <t>754-1123-1-ND</t>
-  </si>
-  <si>
-    <t>LEDs:LED_0603</t>
-  </si>
-  <si>
-    <t>C5,C7,C8,C15</t>
-  </si>
-  <si>
-    <t>C2-C4,C6,
-C9-C14</t>
-  </si>
-  <si>
-    <t>FERRITE BEAD 600 OHM 0603 1LN</t>
-  </si>
-  <si>
-    <t>490-1014-1-ND</t>
-  </si>
-  <si>
-    <t>Resistors_SMD:R_0603</t>
-  </si>
-  <si>
-    <t>RES SMD 470 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>311-470HRCT-ND</t>
-  </si>
-  <si>
-    <t>RES SMD 33 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>311-33.0HRCT-ND</t>
-  </si>
-  <si>
-    <t>SWITCH TACTILE SPST-NO 0.05A 32V</t>
-  </si>
-  <si>
-    <t>CKN10284CT-ND</t>
-  </si>
-  <si>
-    <t>Buttons_Switches_SMD:SW_SPST_KMR2</t>
-  </si>
-  <si>
-    <t>16MHz ±15ppm Crystal 8pF</t>
-  </si>
-  <si>
-    <t>644-1049-1-ND</t>
-  </si>
-  <si>
-    <t>Crystals:Crystal_SMD_2520_4Pads</t>
-  </si>
-  <si>
-    <t>32.768kHz ±20ppm Crystal 12.5pF</t>
-  </si>
-  <si>
-    <t>535-9542-1-ND</t>
-  </si>
-  <si>
-    <t>footprint:ABS07</t>
-  </si>
-  <si>
-    <t>SP1</t>
-  </si>
-  <si>
-    <t>BUZZER PIEZO 12.5V 9MM SMD</t>
-  </si>
-  <si>
-    <t>490-9647-1-ND</t>
-  </si>
-  <si>
-    <t>BT1</t>
-  </si>
-  <si>
-    <t>HOLDER COIN CELL 12MM SMD</t>
-  </si>
-  <si>
-    <t>BK-885-CT-ND</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>568-6524-1-ND</t>
-  </si>
-  <si>
-    <t>DIODE ARRAY SCHOTTKY 40V 3HUSON</t>
-  </si>
-  <si>
-    <t>footprint:PKMCS</t>
-  </si>
-  <si>
-    <t>footprint:BK-885</t>
-  </si>
-  <si>
-    <t>footprint:0855135016</t>
-  </si>
-  <si>
-    <t>USB - micro B USB 2.0 Receptacle</t>
-  </si>
-  <si>
-    <t>609-4613-1-ND</t>
-  </si>
-  <si>
-    <t>footprint:10118192</t>
-  </si>
-  <si>
-    <t>footprint:SOT1061</t>
-  </si>
-  <si>
-    <t>CONN FPC BOTTOM 20POS 1.00MM R/A</t>
-  </si>
-  <si>
-    <t>WM7946CT-ND</t>
-  </si>
-  <si>
-    <t>CABLE FFC 1MM TYPE 2 20P100MM</t>
-  </si>
-  <si>
-    <t>732-5134-ND</t>
-  </si>
-  <si>
-    <t>R1,R4,R5</t>
-  </si>
-  <si>
-    <t>CAP TANT 220UF 16V 10% 2917</t>
-  </si>
-  <si>
-    <t>399-10429-1-ND</t>
-  </si>
-  <si>
-    <t>Capacitors_Tantalum_SMD:TantalC_SizeD_EIA-7343_Reflow</t>
-  </si>
-  <si>
-    <t>footprint:0522712069</t>
-  </si>
-  <si>
-    <t>BATTERY LITHIUM 3V COIN 12.5MM</t>
-  </si>
-  <si>
-    <t>P033-ND</t>
+    <t>IC ADC 24-BIT 10/80SPS 24-TSSOP</t>
+  </si>
+  <si>
+    <t>296-25894-1-ND</t>
+  </si>
+  <si>
+    <t>IC I2C SW 2CH W/RESET 14TSSOP</t>
+  </si>
+  <si>
+    <t>296-42157-1-ND</t>
+  </si>
+  <si>
+    <t>Housings_SSOP:TSSOP-14_4.4x5mm_Pitch0.65mm</t>
+  </si>
+  <si>
+    <t>Housings_SSOP:TSSOP-24_4.4x7.8mm_Pitch0.65mm</t>
+  </si>
+  <si>
+    <t>R6-R13</t>
   </si>
 </sst>
 </file>
@@ -843,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H35"/>
+  <dimension ref="B2:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -886,22 +916,22 @@
     </row>
     <row r="3" spans="2:8">
       <c r="B3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -919,27 +949,27 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="29">
       <c r="B6" s="5" t="s">
-        <v>112</v>
+        <v>155</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>6</v>
@@ -948,30 +978,30 @@
         <v>38</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F7">
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -979,39 +1009,39 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="2:8">
@@ -1022,79 +1052,79 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F14">
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="2:8">
       <c r="B16" t="s">
-        <v>90</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F16">
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -1102,245 +1132,305 @@
     </row>
     <row r="19" spans="2:8">
       <c r="B19" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F19">
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
       <c r="G20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>131</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>121</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
-        <v>100</v>
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>159</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>101</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" t="s">
-        <v>81</v>
+        <v>87</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>102</v>
-      </c>
-      <c r="H28" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="2:8">
       <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
         <v>85</v>
       </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29" t="s">
-        <v>103</v>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" t="s">
-        <v>98</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="6" t="s">
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>119</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C34" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>148</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="2:7">
-      <c r="B35" s="6" t="s">
+      <c r="C37" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C35" t="s">
-        <v>154</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>155</v>
-      </c>
-      <c r="F35">
+      <c r="C38" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>150</v>
+      </c>
+      <c r="F38">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added DC jack for 5V input.  Updated layout
</commit_message>
<xml_diff>
--- a/hardware/beer-gauge-bom.xlsx
+++ b/hardware/beer-gauge-bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="181">
   <si>
     <t>Ref</t>
   </si>
@@ -516,6 +516,51 @@
   </si>
   <si>
     <t>R6-R13</t>
+  </si>
+  <si>
+    <t>CON1</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>CONN PWR JACK 2.0X5.5MM SMD</t>
+  </si>
+  <si>
+    <t>CP-070AHPJCT-ND</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>DIODE ZENER 6.2V 500MW SOD123</t>
+  </si>
+  <si>
+    <t>DDZ6V2BDICT-ND</t>
+  </si>
+  <si>
+    <t>CAP TANT 100UF 10V 20% 2917</t>
+  </si>
+  <si>
+    <t>399-3772-1-ND</t>
+  </si>
+  <si>
+    <t>footprint:PJ-070AH-SMT</t>
+  </si>
+  <si>
+    <t>Diodes_SMD:SOD-123</t>
+  </si>
+  <si>
+    <t>Diodes_SMD:SMA_Standard</t>
+  </si>
+  <si>
+    <t>DIODE GEN PURP 100V 1A SMA</t>
+  </si>
+  <si>
+    <t>S1B-FDICT-ND</t>
   </si>
 </sst>
 </file>
@@ -873,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H38"/>
+  <dimension ref="B2:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -946,202 +991,229 @@
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>145</v>
+        <v>166</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="29">
-      <c r="B6" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>100</v>
-      </c>
+      <c r="E5" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>145</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="29">
+      <c r="B8" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>175</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="D11" s="2"/>
+        <v>147</v>
+      </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>148</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>180</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" t="s">
         <v>93</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C19" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
         <v>109</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="B16" t="s">
-        <v>158</v>
-      </c>
-      <c r="C16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
-      <c r="G16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" t="s">
-        <v>136</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>137</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>112</v>
       </c>
       <c r="F19">
         <v>3</v>
@@ -1150,287 +1222,350 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
-      <c r="B20" t="s">
+    <row r="21" spans="2:7">
+      <c r="B21" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" t="s">
         <v>92</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C25" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
         <v>114</v>
       </c>
-      <c r="F20">
+      <c r="F25">
         <v>2</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G25" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
-      <c r="B21" t="s">
+    <row r="26" spans="2:7">
+      <c r="B26" t="s">
         <v>165</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C26" t="s">
         <v>156</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
         <v>157</v>
       </c>
-      <c r="F21">
+      <c r="F26">
         <v>8</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G26" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" t="s">
+    <row r="27" spans="2:7">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" t="s">
         <v>124</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C28" t="s">
         <v>125</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
         <v>126</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" t="s">
+    <row r="29" spans="2:7">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" t="s">
         <v>94</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C30" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
         <v>116</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
-      <c r="B27" t="s">
+    <row r="32" spans="2:7">
+      <c r="B32" t="s">
         <v>9</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C32" t="s">
         <v>159</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
         <v>160</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="2:8">
-      <c r="B28" t="s">
+    <row r="33" spans="2:8">
+      <c r="B33" t="s">
         <v>79</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C33" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
         <v>86</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="2:8">
-      <c r="B29" t="s">
+    <row r="34" spans="2:8">
+      <c r="B34" t="s">
         <v>80</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C34" t="s">
         <v>82</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D34" t="s">
         <v>81</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E34" t="s">
         <v>83</v>
       </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
         <v>98</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H34" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
-      <c r="B30" t="s">
+    <row r="35" spans="2:8">
+      <c r="B35" t="s">
         <v>21</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C35" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
         <v>85</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="2:8">
-      <c r="B31" t="s">
+    <row r="36" spans="2:8">
+      <c r="B36" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C36" t="s">
         <v>161</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
         <v>162</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="2:8">
-      <c r="B32" t="s">
+    <row r="37" spans="2:8">
+      <c r="B37" t="s">
         <v>151</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C37" t="s">
         <v>152</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
         <v>153</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
-      <c r="B34" t="s">
+    <row r="39" spans="2:8">
+      <c r="B39" t="s">
         <v>95</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C39" t="s">
         <v>118</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
         <v>119</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
-      <c r="B35" t="s">
+    <row r="40" spans="2:8">
+      <c r="B40" t="s">
         <v>96</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C40" t="s">
         <v>121</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
         <v>122</v>
       </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="2:7">
-      <c r="B37" s="6" t="s">
+    <row r="42" spans="2:8">
+      <c r="B42" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C42" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
         <v>143</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="2:7">
-      <c r="B38" s="6" t="s">
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C43" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
         <v>150</v>
       </c>
-      <c r="F38">
+      <c r="F43">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated BOM with sensor board parts
</commit_message>
<xml_diff>
--- a/hardware/beer-gauge-bom.xlsx
+++ b/hardware/beer-gauge-bom.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8020" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Main Board" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensor Board" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="131">
   <si>
     <t>Ref</t>
   </si>
@@ -38,222 +38,34 @@
     <t>DigiKey</t>
   </si>
   <si>
-    <t>http://www.ti.com/product/ads1131/description</t>
-  </si>
-  <si>
-    <t>http://www.microchip.com/wwwproducts/Devices.aspx?product=PIC24FJ128GB202</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
-    <t>U2,U3</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>CONN HEADER 10POS DL UNSHRD SMD</t>
-  </si>
-  <si>
-    <t>609-3729-ND</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>CONN MINI USB RCPT RA TYPE B SMD</t>
-  </si>
-  <si>
-    <t>609-4700-1-ND</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
-    <t>LED BLUE CLEAR 0805 SMD</t>
-  </si>
-  <si>
-    <t>160-1579-1-ND</t>
-  </si>
-  <si>
-    <t>J3,J4</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
-    <t>IC SENSOR THERMAL 3.1V SOT-23-3</t>
-  </si>
-  <si>
-    <t>MCP9701T-E/TTCT-ND</t>
-  </si>
-  <si>
-    <t>IC REG LDO 3.3V 0.3A SOT223-3</t>
-  </si>
-  <si>
-    <t>TC1108-3.3VDBTRCT-ND</t>
-  </si>
-  <si>
-    <t>SM/SOT223_1234</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
-    <t>J5,J6</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
-    <t>CAP CER 10UF 6.3V 10% X5R 0805</t>
-  </si>
-  <si>
-    <t>311-1459-1-ND</t>
-  </si>
-  <si>
-    <t>CAP CER 1UF 10V 10% X5R 0603</t>
-  </si>
-  <si>
-    <t>311-1443-1-ND</t>
-  </si>
-  <si>
     <t>Footprint</t>
   </si>
   <si>
-    <t>SM/C_0603</t>
-  </si>
-  <si>
-    <t>SM/C_0805</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 25V 10% X7R 0603</t>
-  </si>
-  <si>
     <t>311-1341-1-ND</t>
   </si>
   <si>
-    <t>C8,C9</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>C2,C3,C5,C6,
-C10,C11</t>
-  </si>
-  <si>
-    <t>20021121-00010T4LF</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
     <t>R3,R4</t>
-  </si>
-  <si>
-    <t>RES 10.0K OHM 1/10W 1% 0603 SMD</t>
-  </si>
-  <si>
-    <t>311-10.0KHRCT-ND</t>
-  </si>
-  <si>
-    <t>SM/R_0603</t>
-  </si>
-  <si>
-    <t>RES 100 OHM 1/10W 1% 0603 SMD</t>
-  </si>
-  <si>
-    <t>311-100HRCT-ND</t>
-  </si>
-  <si>
-    <t>SM/SOT23_123</t>
-  </si>
-  <si>
-    <t>SM/D_0805_21</t>
-  </si>
-  <si>
-    <t>10033526-N3212LF</t>
-  </si>
-  <si>
-    <t>HEADER3X1</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>FB1</t>
-  </si>
-  <si>
-    <t>FERRITE CHIP POWER 600 OHM SMD</t>
-  </si>
-  <si>
-    <t>240-2390-1-ND</t>
-  </si>
-  <si>
-    <t>SM/R_0805</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>C4,C7,C12,C13,
-C14,C16</t>
-  </si>
-  <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>CAP TANT 4.7UF 16V 20% 1206</t>
-  </si>
-  <si>
-    <t>399-3699-1-ND</t>
-  </si>
-  <si>
-    <t>SM/C_1206</t>
-  </si>
-  <si>
-    <t>CAP CER 10000PF 50V 10% X7R 0603</t>
-  </si>
-  <si>
-    <t>311-1572-1-ND</t>
-  </si>
-  <si>
-    <t>RES 330 OHM 1/10W 1% 0603 SMD</t>
-  </si>
-  <si>
-    <t>311-330HRCT-ND</t>
-  </si>
-  <si>
-    <t>CONN MOD JACK R/A 4P4C</t>
-  </si>
-  <si>
-    <t>609-1054-ND</t>
-  </si>
-  <si>
-    <t>87180-044LF</t>
-  </si>
-  <si>
-    <t>PIC24FJ128GB202-I/SS-ND</t>
-  </si>
-  <si>
-    <t>IC MCU 16BIT 128KB FLASH 28SSOP</t>
-  </si>
-  <si>
-    <t>PIC24FJ128GB202-I/SS</t>
-  </si>
-  <si>
-    <t>IC ADC 18BIT DELTA-SIG 16TSSOP</t>
-  </si>
-  <si>
-    <t>296-24612-5-ND</t>
-  </si>
-  <si>
-    <t>ADS1130</t>
   </si>
   <si>
     <t>U2</t>
@@ -561,6 +373,42 @@
   </si>
   <si>
     <t>S1B-FDICT-ND</t>
+  </si>
+  <si>
+    <t>C1,C2</t>
+  </si>
+  <si>
+    <t>C3,C4</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>SENSOR PRESSURE 30 PSIG</t>
+  </si>
+  <si>
+    <t>480-6247-ND</t>
+  </si>
+  <si>
+    <t>SENSOR TEMP I2C/SMBUS 8DFN</t>
+  </si>
+  <si>
+    <t>MCP9808T-E/MCCT-ND</t>
+  </si>
+  <si>
+    <t>Monochrome 2.42" 128x64 OLED Graphic Display Module Kit</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2719</t>
+  </si>
+  <si>
+    <t>CONN MOD JACK 4P4C R/A UNSHLD</t>
+  </si>
+  <si>
+    <t>WM3544CT-ND</t>
   </si>
 </sst>
 </file>
@@ -604,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -616,6 +464,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,18 +769,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H43"/>
+  <dimension ref="B2:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="2.6328125" customWidth="1"/>
     <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46.6328125" bestFit="1" customWidth="1"/>
@@ -953,7 +804,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
@@ -961,22 +812,22 @@
     </row>
     <row r="3" spans="2:8">
       <c r="B3" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>128</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>134</v>
+        <v>72</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -991,22 +842,22 @@
     </row>
     <row r="5" spans="2:8">
       <c r="B5" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>169</v>
+        <v>107</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>170</v>
+        <v>108</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>176</v>
+        <v>114</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -1021,162 +872,162 @@
     </row>
     <row r="7" spans="2:8">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>147</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="29">
       <c r="B8" s="5" t="s">
-        <v>155</v>
+        <v>93</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" t="s">
-        <v>168</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>112</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>175</v>
+        <v>113</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>147</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:8">
       <c r="B13" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>139</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>110</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>173</v>
+        <v>111</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>177</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="C15" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>180</v>
+        <v>118</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -1184,82 +1035,82 @@
     </row>
     <row r="17" spans="2:7">
       <c r="B17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>79</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>148</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="F19">
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" t="s">
-        <v>158</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="F21">
         <v>4</v>
       </c>
       <c r="G21" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>138</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="2:7">
@@ -1267,62 +1118,62 @@
     </row>
     <row r="24" spans="2:7">
       <c r="B24" t="s">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="F24">
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" t="s">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>52</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" t="s">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>94</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>157</v>
+        <v>95</v>
       </c>
       <c r="F26">
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="2:7">
@@ -1330,22 +1181,22 @@
     </row>
     <row r="28" spans="2:7">
       <c r="B28" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="2:7">
@@ -1353,199 +1204,199 @@
     </row>
     <row r="30" spans="2:7">
       <c r="B30" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="2:7">
       <c r="B32" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>159</v>
+        <v>97</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>160</v>
+        <v>98</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>164</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="2:8">
       <c r="B34" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="H34" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E35" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>161</v>
+        <v>99</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>162</v>
+        <v>100</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>163</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="2:8">
       <c r="B37" t="s">
-        <v>151</v>
+        <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>152</v>
+        <v>90</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>153</v>
+        <v>91</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>154</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="2:8">
       <c r="B39" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>119</v>
+        <v>57</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>120</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="2:8">
       <c r="B40" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>123</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="2:8">
       <c r="B42" s="6" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>143</v>
+        <v>81</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1554,19 +1405,39 @@
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="6" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>149</v>
+        <v>87</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>150</v>
+        <v>88</v>
       </c>
       <c r="F43">
         <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" t="s">
+        <v>127</v>
+      </c>
+      <c r="E44" s="7">
+        <v>2719</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1577,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H27"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G21" sqref="G20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1611,135 +1482,103 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:8">
-      <c r="B3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="2:8" ht="29">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:8">
+      <c r="B4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="2">
-        <v>6</v>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:8" ht="29">
-      <c r="B5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="2">
-        <v>6</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>35</v>
-      </c>
+    <row r="5" spans="2:8">
+      <c r="B5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="2" t="s">
-        <v>39</v>
+      <c r="B6" t="s">
+        <v>121</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>40</v>
+        <v>129</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -1753,53 +1592,60 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="2" t="s">
-        <v>56</v>
+      <c r="B12" t="s">
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>59</v>
+        <v>123</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -1813,87 +1659,38 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>42</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="2">
-        <v>2</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="2">
-        <v>2</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="2:8">
@@ -1906,87 +1703,35 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>48</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>48</v>
-      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="2:8">
-      <c r="B21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="2">
-        <v>2</v>
-      </c>
-      <c r="G21" t="s">
-        <v>48</v>
-      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>48</v>
-      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="2"/>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="2:8">
@@ -1999,90 +1744,12 @@
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="2">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27" t="s">
-        <v>26</v>
-      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>